<commit_message>
SVD e Sistemas dinâmicos acrescentados. Arquivos do Gastão atualizados.
</commit_message>
<xml_diff>
--- a/Biblioteca de ALC (organizada pelo gastão).xlsx
+++ b/Biblioteca de ALC (organizada pelo gastão).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/408a87062437540a/Documentos pessoais/Cursos/Doutorado - O retorno/2020.1 Álgebra linear computacional/Biblioteca/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gasta\biblioteca_algebra_linear_ppgi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_8ECC0C6ED608D71AC6F30DB4C43340A64E52DD2C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{16F1D5CF-0129-4B38-A0CB-945E126ACACD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5075147D-F02A-4918-BD6F-81BC1502DB24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="12630" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16080" yWindow="12900" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1328,10 +1328,10 @@
   <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1348,7 +1348,7 @@
     <col min="10" max="10" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1394,7 +1394,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1404,7 +1404,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1413,7 +1413,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1433,25 +1433,25 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>151</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>146</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>142</v>
@@ -1460,28 +1460,28 @@
         <v>33</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>151</v>
+        <v>144</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>146</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>142</v>
@@ -1490,10 +1490,10 @@
         <v>33</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>164</v>
       </c>
@@ -1504,7 +1504,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>25</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>139</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>29</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>34</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>39</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>43</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>49</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>61</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>65</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>68</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>74</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>101</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>58</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>90</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>94</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>123</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>125</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>128</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>80</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>85</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>20</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>79</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>156</v>
       </c>
@@ -2035,7 +2035,7 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>97</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>103</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>116</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>120</v>
       </c>
@@ -2114,7 +2114,7 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>132</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
         <v>136</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>112</v>
       </c>
@@ -2258,29 +2258,29 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="19"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="20"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="19"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="19"/>
     </row>
   </sheetData>

</xml_diff>